<commit_message>
Minnor changes in OpenSource results
</commit_message>
<xml_diff>
--- a/results/OpenSource Tools/C - OpenSource tools (LICCA).xlsx
+++ b/results/OpenSource Tools/C - OpenSource tools (LICCA).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PREBACIVANJE (D)\UROS - IT\PMF\MASTER\Napredne teme softverskog inženjerstva\Seminarski rad\OpenSource Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PREBACIVANJE (D)\UROS - IT\PMF\MASTER\Napredne teme softverskog inženjerstva\Seminarski rad\results\OpenSource Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AA63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N58" sqref="N58"/>
+    <sheetView tabSelected="1" topLeftCell="K22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2212,28 +2212,28 @@
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="T32" s="13">
-        <f>_xlfn.STDEV.S(C29,M29)</f>
-        <v>39.952318811241256</v>
+        <f>_xlfn.STDEV.P(C29,M29)</f>
+        <v>28.250555555555557</v>
       </c>
       <c r="U32" s="9">
-        <f>_xlfn.STDEV.S(E29,N29)</f>
-        <v>13.985000783467273</v>
+        <f>_xlfn.STDEV.P(E29,N29)</f>
+        <v>9.8888888888888893</v>
       </c>
       <c r="V32" s="9">
-        <f>_xlfn.STDEV.S(F29,O29)</f>
-        <v>322.18220540883186</v>
+        <f>_xlfn.STDEV.P(F29,O29)</f>
+        <v>227.8172222222222</v>
       </c>
       <c r="W32" s="9">
-        <f>_xlfn.STDEV.S(H29,Q29)</f>
-        <v>11.879786761034657</v>
+        <f>_xlfn.STDEV.P(H29,Q29)</f>
+        <v>8.4002777777777773</v>
       </c>
       <c r="X32" s="9">
-        <f>_xlfn.STDEV.S(L29,S29)</f>
-        <v>0.78567420131838617</v>
+        <f>_xlfn.STDEV.P(L29,S29)</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="Y32" s="9">
-        <f>_xlfn.STDEV.S(J29,R29)</f>
-        <v>14.764602552358518</v>
+        <f>_xlfn.STDEV.P(J29,R29)</f>
+        <v>10.440150586296916</v>
       </c>
       <c r="Z32" s="9"/>
       <c r="AA32" s="25" t="s">
@@ -2242,28 +2242,28 @@
     </row>
     <row r="33" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T33" s="13">
-        <f>_xlfn.VAR.S(C29,M29)</f>
-        <v>1596.1877783950617</v>
+        <f>_xlfn.VAR.P(C29,M29)</f>
+        <v>798.09388919753087</v>
       </c>
       <c r="U33" s="9">
-        <f>_xlfn.VAR.S(E29,N29)</f>
-        <v>195.58024691358025</v>
+        <f>_xlfn.VAR.P(E29,N29)</f>
+        <v>97.790123456790127</v>
       </c>
       <c r="V33" s="9">
-        <f>_xlfn.VAR.S(F29,O29)</f>
-        <v>103801.37348209874</v>
+        <f>_xlfn.VAR.P(F29,O29)</f>
+        <v>51900.686741049372</v>
       </c>
       <c r="W33" s="9">
-        <f>_xlfn.VAR.S(H29,Q29)</f>
-        <v>141.12933348765429</v>
+        <f>_xlfn.VAR.P(H29,Q29)</f>
+        <v>70.564666743827146</v>
       </c>
       <c r="X33" s="9">
-        <f>_xlfn.VAR.S(L29,S29)</f>
-        <v>0.61728395061728403</v>
+        <f>_xlfn.VAR.P(L29,S29)</f>
+        <v>0.30864197530864201</v>
       </c>
       <c r="Y33" s="9">
-        <f>_xlfn.VAR.S(J29,R29)</f>
-        <v>217.99348852911169</v>
+        <f>_xlfn.VAR.P(J29,R29)</f>
+        <v>108.99674426455584</v>
       </c>
       <c r="Z33" s="9"/>
       <c r="AA33" s="25" t="s">
@@ -2956,20 +2956,20 @@
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K61" s="13">
-        <f>_xlfn.STDEV.S(C58,G58)</f>
-        <v>6.7567981313381207</v>
+        <f>_xlfn.STDEV.P(C58,G58)</f>
+        <v>4.7777777777777777</v>
       </c>
       <c r="L61" s="9">
-        <f>_xlfn.STDEV.S(D58,H58)</f>
-        <v>7.2282026521291547</v>
+        <f>_xlfn.STDEV.P(D58,H58)</f>
+        <v>5.1111111111111125</v>
       </c>
       <c r="M61" s="9">
-        <f t="shared" ref="M61:N61" si="11">_xlfn.STDEV.S(E58,I58)</f>
-        <v>19.209734222234541</v>
+        <f>_xlfn.STDEV.P(E58,I58)</f>
+        <v>13.583333333333332</v>
       </c>
       <c r="N61" s="9">
-        <f t="shared" si="11"/>
-        <v>24.709453631463244</v>
+        <f>_xlfn.STDEV.P(F58,J58)</f>
+        <v>17.472222222222221</v>
       </c>
       <c r="O61" s="9"/>
       <c r="P61" s="25" t="s">
@@ -2978,20 +2978,20 @@
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K62" s="13">
-        <f>_xlfn.VAR.S(C58,G58)</f>
-        <v>45.654320987654316</v>
+        <f>_xlfn.VAR.P(C58,G58)</f>
+        <v>22.827160493827158</v>
       </c>
       <c r="L62" s="9">
-        <f>_xlfn.VAR.S(D58,H58)</f>
-        <v>52.24691358024694</v>
+        <f>_xlfn.VAR.P(D58,H58)</f>
+        <v>26.12345679012347</v>
       </c>
       <c r="M62" s="9">
-        <f t="shared" ref="M62:N62" si="12">_xlfn.VAR.S(E58,I58)</f>
-        <v>369.01388888888886</v>
+        <f>_xlfn.VAR.P(E58,I58)</f>
+        <v>184.50694444444443</v>
       </c>
       <c r="N62" s="9">
-        <f t="shared" si="12"/>
-        <v>610.5570987654321</v>
+        <f>_xlfn.VAR.P(F58,J58)</f>
+        <v>305.27854938271605</v>
       </c>
       <c r="O62" s="9"/>
       <c r="P62" s="25" t="s">

</xml_diff>